<commit_message>
added documentation. gerber of v1.0.0
</commit_message>
<xml_diff>
--- a/VGA Timing.xlsx
+++ b/VGA Timing.xlsx
@@ -7,8 +7,10 @@
   </bookViews>
   <sheets>
     <sheet name="Display 800x600" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Display 640x480" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Display 640x480 @ 60hZ big" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Display 640x480 @ 60hZ" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Display 640x480 @ 85Hz" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -18,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">Design Clock (MHz)</t>
   </si>
@@ -101,6 +103,9 @@
     <t>width</t>
   </si>
   <si>
+    <t xml:space="preserve">% drawing</t>
+  </si>
+  <si>
     <t>height</t>
   </si>
   <si>
@@ -125,16 +130,49 @@
     <t xml:space="preserve">A7-A13 Y Coord</t>
   </si>
   <si>
+    <t xml:space="preserve">pld clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pixel clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 bit x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 bit y</t>
+  </si>
+  <si>
     <t xml:space="preserve">EFFECTIVE RESOLUTION</t>
   </si>
   <si>
-    <t>203x120</t>
+    <t>407x240</t>
   </si>
   <si>
     <t xml:space="preserve">Pixel (8bit)</t>
   </si>
   <si>
     <t>bytes</t>
+  </si>
+  <si>
+    <t>203x120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 bit x</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">427x240 px @85hz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspect ratio</t>
   </si>
   <si>
     <t xml:space="preserve">Address Calculator</t>
@@ -177,7 +215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +224,12 @@
     </fill>
     <fill>
       <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -219,7 +263,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -235,26 +279,19 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -850,11 +887,12 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <f>B1/B2</f>
+        <v>5</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E9" si="0">B6/D6</f>
-        <v>266.66666666666669</v>
+        <v>160</v>
       </c>
       <c r="F6">
         <v>160</v>
@@ -883,11 +921,12 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <f>B1/B2</f>
+        <v>5</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -916,11 +955,12 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <f>B1/B2</f>
+        <v>5</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>42.666666666666664</v>
+        <v>25.600000000000001</v>
       </c>
       <c r="F8">
         <v>25</v>
@@ -949,11 +989,12 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <f>B1/B2</f>
+        <v>5</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>29.333333333333332</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F9">
         <v>18</v>
@@ -982,11 +1023,12 @@
         <v>26.399999999999999</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <f>B1/B2</f>
+        <v>5</v>
       </c>
       <c r="E10" s="4">
         <f>B10/D10</f>
-        <v>352</v>
+        <v>211.19999999999999</v>
       </c>
       <c r="F10">
         <f>SUM(F6:F9)</f>
@@ -1037,11 +1079,11 @@
         <v>15.84</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" ref="E14:E18" si="3">B14/D14</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="F14">
         <v>120</v>
@@ -1066,11 +1108,11 @@
         <v>0.0264</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1095,11 +1137,11 @@
         <v>0.1056</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1124,11 +1166,11 @@
         <v>0.60719999999999996</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="3"/>
-        <v>11.5</v>
+        <v>5.75</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -1153,11 +1195,11 @@
         <v>16.5792</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="3"/>
-        <v>314</v>
+        <v>157</v>
       </c>
       <c r="F18" s="4">
         <f>SUM(F14:F17)</f>
@@ -1202,10 +1244,17 @@
       <c r="D23">
         <v>0</v>
       </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="7">
+        <f>(C6*B14)/(C18*1000)</f>
+        <v>0.72379849449913136</v>
+      </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>120</v>
@@ -1219,7 +1268,7 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>332</v>
@@ -1262,7 +1311,7 @@
     </row>
     <row r="32" ht="14.25">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -1271,7 +1320,7 @@
         <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" ht="14.25">
@@ -1288,13 +1337,13 @@
         <f>B33*B34</f>
         <v>5504</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>31</v>
+      <c r="G33" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34">
         <v>64</v>
@@ -1303,23 +1352,22 @@
         <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35"/>
       <c r="D35">
         <v>8</v>
       </c>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" ht="14.25">
@@ -1416,23 +1464,33 @@
       </c>
       <c r="D6">
         <f>B1/B2</f>
-        <v>3.1468750000000001</v>
+        <v>1.5734375</v>
       </c>
       <c r="E6">
         <f>B6/D6</f>
-        <v>203.37636544190664</v>
+        <v>406.75273088381329</v>
       </c>
       <c r="F6" s="3">
         <f>ROUND(E6,0)</f>
-        <v>203</v>
+        <v>407</v>
       </c>
       <c r="G6" s="3">
         <f>F6/B2</f>
-        <v>25.375</v>
+        <v>25.4375</v>
       </c>
       <c r="H6">
         <f>(G6-C6)/C6</f>
-        <v>-0.0018505859281423528</v>
+        <v>0.0006079101656306956</v>
+      </c>
+      <c r="J6" t="str">
+        <f>DEC2HEX(F6)</f>
+        <v>197</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1447,15 +1505,15 @@
       </c>
       <c r="D7" s="4">
         <f>B1/B2</f>
-        <v>3.1468750000000001</v>
+        <v>1.5734375</v>
       </c>
       <c r="E7" s="4">
         <f>B7/D7</f>
-        <v>5.0844091360476664</v>
+        <v>10.168818272095333</v>
       </c>
       <c r="F7" s="5">
         <f>ROUND(E7,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G7" s="5">
         <f>F7/B2</f>
@@ -1465,6 +1523,16 @@
         <f>(G7-C7)/C7</f>
         <v>-0.03183497015185946</v>
       </c>
+      <c r="J7" s="4" t="str">
+        <f>DEC2HEX(F7+J6)</f>
+        <v>CF</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
@@ -1478,25 +1546,31 @@
       </c>
       <c r="D8" s="4">
         <f>B1/B2</f>
-        <v>3.1468750000000001</v>
+        <v>1.5734375</v>
       </c>
       <c r="E8" s="4">
         <f>B8/D8</f>
-        <v>30.506454816285999</v>
+        <v>61.012909632571997</v>
       </c>
       <c r="F8" s="5">
         <f>ROUND(E8,0)</f>
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="G8" s="5">
         <f>F8/B2</f>
-        <v>3.875</v>
+        <v>3.8125</v>
       </c>
       <c r="H8" s="6">
         <f>(G8-C8)/C8</f>
-        <v>0.01617839928326777</v>
+        <v>-0.00021157489872041909</v>
       </c>
       <c r="I8" s="4"/>
+      <c r="J8" t="str">
+        <f>DEC2HEX(F6+F7+F8)</f>
+        <v>1DE</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
@@ -1510,25 +1584,31 @@
       </c>
       <c r="D9" s="4">
         <f>B1/B2</f>
-        <v>3.1468750000000001</v>
+        <v>1.5734375</v>
       </c>
       <c r="E9" s="4">
         <f>B9/D9</f>
-        <v>15.253227408142999</v>
+        <v>30.506454816285999</v>
       </c>
       <c r="F9" s="5">
         <f>ROUND(E9,0)</f>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G9" s="5">
         <f>F9/B2</f>
-        <v>1.875</v>
+        <v>1.9375</v>
       </c>
       <c r="H9" s="6">
         <f>(G9-C9)/C9</f>
-        <v>-0.01660154908070861</v>
+        <v>0.01617839928326777</v>
       </c>
       <c r="I9" s="4"/>
+      <c r="J9" t="str">
+        <f>DEC2HEX(F6+F7+F8+F9)</f>
+        <v>1FD</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
@@ -1544,15 +1624,15 @@
       </c>
       <c r="D10" s="4">
         <f>B1/B2</f>
-        <v>3.1468750000000001</v>
+        <v>1.5734375</v>
       </c>
       <c r="E10" s="4">
         <f>B10/D10</f>
-        <v>254.2204568023833</v>
+        <v>508.44091360476659</v>
       </c>
       <c r="F10" s="5">
         <f>ROUND(E10,0)</f>
-        <v>254</v>
+        <v>508</v>
       </c>
       <c r="G10" s="5">
         <f>F10/B2</f>
@@ -1563,9 +1643,13 @@
         <v>-0.0011814994157502558</v>
       </c>
       <c r="I10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" ht="14.25">
       <c r="F11" s="3"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="2" t="s">
@@ -1576,6 +1660,8 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
@@ -1592,6 +1678,8 @@
       </c>
       <c r="F13" s="3"/>
       <c r="H13" s="6"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
@@ -1605,15 +1693,15 @@
         <v>15.258027350399999</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" s="4">
         <f>B14/D14</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="F14" s="5">
         <f>ROUND(E14,0)</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="G14" s="3">
         <f>F14/B2</f>
@@ -1623,6 +1711,12 @@
         <f>(G14-C14)/C14</f>
         <v>-0.016910924621801434</v>
       </c>
+      <c r="J14" t="str">
+        <f>DEC2HEX(B14)</f>
+        <v>1E0</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
@@ -1636,24 +1730,29 @@
         <v>0.31787556979999998</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="4">
         <f>B15/D15</f>
-        <v>2.5</v>
-      </c>
-      <c r="F15" s="5">
-        <f>E15</f>
-        <v>2.5</v>
+        <v>5</v>
+      </c>
+      <c r="F15" s="9">
+        <v>7</v>
       </c>
       <c r="G15" s="5">
         <f>F15/B2</f>
-        <v>0.3125</v>
+        <v>0.4375</v>
       </c>
       <c r="H15" s="6">
         <f>(G15-C15)*100/C15</f>
-        <v>-1.6910924621801433</v>
-      </c>
+        <v>37.632470552947801</v>
+      </c>
+      <c r="J15" t="str">
+        <f>DEC2HEX(B15+B14)</f>
+        <v>1EA</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
@@ -1667,23 +1766,32 @@
         <v>0.063575113959999999</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="4">
         <f>B16/D16</f>
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="5">
-        <f>E16</f>
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>2</v>
       </c>
       <c r="G16" s="5">
         <f>F16/B2</f>
-        <v>0.0625</v>
+        <v>0.125</v>
       </c>
       <c r="H16" s="6">
         <f>(G16-C16)/C16</f>
-        <v>-0.016910924621801476</v>
+        <v>0.96617815075639701</v>
+      </c>
+      <c r="J16" t="str">
+        <f>DEC2HEX(B16+B15+B14)</f>
+        <v>1EC</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="14.25">
@@ -1698,15 +1806,15 @@
         <v>1.0489893803400001</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17" s="4">
         <f>B17/D17</f>
-        <v>8.25</v>
+        <v>16.5</v>
       </c>
       <c r="F17" s="5">
         <f>E17</f>
-        <v>8.25</v>
+        <v>16.5</v>
       </c>
       <c r="G17" s="5">
         <f>F17/B2</f>
@@ -1716,6 +1824,10 @@
         <f>(G17-C17)/C17</f>
         <v>-0.016910924621801601</v>
       </c>
+      <c r="J17" t="str">
+        <f>DEC2HEX(B14+B15+B16+B17)</f>
+        <v>20D</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
@@ -1730,86 +1842,84 @@
         <v>16.6884674145</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18" s="4">
         <f>B18/D18</f>
-        <v>131.25</v>
+        <v>262.5</v>
       </c>
       <c r="F18" s="5">
         <f>SUM(F14:F17)</f>
-        <v>131.25</v>
+        <v>265.5</v>
       </c>
       <c r="G18" s="5">
         <f>F18/B2</f>
-        <v>16.40625</v>
+        <v>16.59375</v>
       </c>
       <c r="H18" s="6">
         <f>(G18-C18)/C18</f>
-        <v>-0.016910924621801486</v>
+        <v>-0.0056756209031935019</v>
       </c>
     </row>
     <row r="20" ht="14.25"/>
-    <row r="21" ht="14.25">
-      <c r="K21" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="21" ht="14.25"/>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="7">
+        <f>(C6*B14)/(C18*1000)</f>
+        <v>0.73119847516960268</v>
       </c>
     </row>
     <row r="24" ht="14.25"/>
     <row r="25" ht="14.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B25">
-        <f>203*120</f>
-        <v>24360</v>
+        <f>407*240</f>
+        <v>97680</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26">
+        <f>2^17</f>
+        <v>131072</v>
+      </c>
+    </row>
     <row r="27" ht="14.25"/>
     <row r="28" ht="14.25"/>
     <row r="30" ht="14.25"/>
-    <row r="32" ht="14.25">
-      <c r="C32"/>
-      <c r="D32"/>
-    </row>
+    <row r="32" ht="14.25"/>
     <row r="33" ht="14.25">
-      <c r="A33"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" ht="14.25">
-      <c r="A34"/>
-    </row>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" ht="14.25"/>
     <row r="35" ht="14.25">
-      <c r="A35"/>
       <c r="D35">
         <v>8</v>
       </c>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1832,121 +1942,1193 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.7109375"/>
+    <col customWidth="1" min="5" max="5" width="13.140625"/>
+    <col customWidth="1" min="7" max="7" width="15.8515625"/>
+    <col bestFit="1" min="8" max="8" width="10.65234375"/>
+  </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="K1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="8"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>25.175000000000001</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="K3" s="9" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>640</v>
+      </c>
+      <c r="C6" s="3">
+        <v>25.42204568</v>
+      </c>
+      <c r="D6">
+        <f>B1/B2</f>
+        <v>3.1468750000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E9" si="5">B6/D6</f>
+        <v>203.37636544190664</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" ref="F6:F9" si="6">ROUND(E6,0)</f>
+        <v>203</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6/B2</f>
+        <v>25.375</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H9" si="7">(G6-C6)/C6</f>
+        <v>-0.0018505859281423528</v>
+      </c>
+      <c r="J6" t="str">
+        <f>DEC2HEX(F6)</f>
+        <v>CB</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.64555110000000004</v>
+      </c>
+      <c r="D7" s="4">
+        <f>B1/B2</f>
+        <v>3.1468750000000001</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="5"/>
+        <v>5.0844091360476664</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="5">
+        <f>F7/B2</f>
+        <v>0.625</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="7"/>
+        <v>-0.03183497015185946</v>
+      </c>
+      <c r="J7" s="4" t="e">
+        <f>DEC2HEX(F7+J6)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>96</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.8133067999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <f>B1/B2</f>
+        <v>3.1468750000000001</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="5"/>
+        <v>30.506454816285999</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="G8" s="5">
+        <f>F8/B2</f>
+        <v>3.875</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="7"/>
+        <v>0.01617839928326777</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" t="str">
+        <f>DEC2HEX(F6+F7+F8)</f>
+        <v>EF</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>48</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.9066533999999999</v>
+      </c>
+      <c r="D9" s="4">
+        <f>B1/B2</f>
+        <v>3.1468750000000001</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="5"/>
+        <v>15.253227408142999</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="G9" s="5">
+        <f>F9/B2</f>
+        <v>1.875</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="7"/>
+        <v>-0.01660154908070861</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" t="str">
+        <f>DEC2HEX(F6+F7+F8+F9)</f>
+        <v>FE</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B6:B9)</f>
+        <v>800</v>
+      </c>
+      <c r="C10" s="3">
+        <f>SUM(C6:C9)</f>
+        <v>31.787556979999998</v>
+      </c>
+      <c r="D10" s="4">
+        <f>B1/B2</f>
+        <v>3.1468750000000001</v>
+      </c>
+      <c r="E10" s="4">
+        <f>B10/D10</f>
+        <v>254.2204568023833</v>
+      </c>
+      <c r="F10" s="5">
+        <f>ROUND(E10,0)</f>
+        <v>254</v>
+      </c>
+      <c r="G10" s="5">
+        <f>F10/B2</f>
+        <v>31.75</v>
+      </c>
+      <c r="H10" s="6">
+        <f>(G10-C10)/C10</f>
+        <v>-0.0011814994157502558</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>480</v>
+      </c>
+      <c r="C14">
+        <f>C10*B14/1000</f>
+        <v>15.258027350399999</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" ref="E14:E18" si="8">B14/D14</f>
+        <v>120</v>
+      </c>
+      <c r="F14" s="5">
+        <f>ROUND(E14,0)</f>
+        <v>120</v>
+      </c>
+      <c r="G14" s="3">
+        <f>F14/B2</f>
+        <v>15</v>
+      </c>
+      <c r="H14" s="6">
+        <f>(G14-C14)/C14</f>
+        <v>-0.016910924621801434</v>
+      </c>
+      <c r="J14" t="str">
+        <f>DEC2HEX(B14)</f>
+        <v>1E0</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <f>C10*B15/1000</f>
+        <v>0.31787556979999998</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" ref="F15:F17" si="9">E15</f>
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="5">
+        <f>F15/B2</f>
+        <v>0.3125</v>
+      </c>
+      <c r="H15" s="6">
+        <f>(G15-C15)*100/C15</f>
+        <v>-1.6910924621801433</v>
+      </c>
+      <c r="J15" t="str">
+        <f>DEC2HEX(B15+B14)</f>
+        <v>1EA</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <f>C10*B16/1000</f>
+        <v>0.063575113959999999</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="5">
+        <f>F16/B2</f>
+        <v>0.0625</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" ref="H16:H18" si="10">(G16-C16)/C16</f>
+        <v>-0.016910924621801476</v>
+      </c>
+      <c r="J16" t="str">
+        <f>DEC2HEX(B16+B15+B14)</f>
+        <v>1EC</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <f>C10*B17/1000</f>
+        <v>1.0489893803400001</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="8"/>
+        <v>8.25</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="9"/>
+        <v>8.25</v>
+      </c>
+      <c r="G17" s="5">
+        <f>F17/B2</f>
+        <v>1.03125</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="10"/>
+        <v>-0.016910924621801601</v>
+      </c>
+      <c r="J17" t="str">
+        <f>DEC2HEX(B14+B15+B16+B17)</f>
+        <v>20D</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B14:B17)</f>
+        <v>525</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C14:C17)</f>
+        <v>16.6884674145</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="8"/>
+        <v>131.25</v>
+      </c>
+      <c r="F18" s="5">
+        <f>SUM(F14:F17)</f>
+        <v>131.25</v>
+      </c>
+      <c r="G18" s="5">
+        <f>F18/B2</f>
+        <v>16.40625</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="10"/>
+        <v>-0.016910924621801486</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25"/>
+    <row r="21" ht="14.25">
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="7">
+        <f>(C6*B14)/(C18*1000)</f>
+        <v>0.73119847516960268</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25"/>
+    <row r="25" ht="14.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <f>203*120</f>
+        <v>24360</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25"/>
+    <row r="27" ht="14.25"/>
+    <row r="28" ht="14.25"/>
+    <row r="30" ht="14.25"/>
+    <row r="32" ht="14.25"/>
+    <row r="33" ht="14.25">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" ht="14.25"/>
+    <row r="35" ht="14.25">
+      <c r="D35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A12:E12"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.7109375"/>
+    <col customWidth="1" min="5" max="5" width="13.140625"/>
+    <col customWidth="1" min="7" max="7" width="15.8515625"/>
+    <col bestFit="1" min="8" max="8" width="10.65234375"/>
+    <col customWidth="1" min="10" max="10" width="11.00390625"/>
+    <col customWidth="1" min="12" max="12" width="11.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>640</v>
+      </c>
+      <c r="C6" s="3">
+        <v>17.777699999999999</v>
+      </c>
+      <c r="D6">
+        <f>B1/B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E9" si="11">B6/D6</f>
+        <v>426.66666666666669</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" ref="F6:F9" si="12">ROUND(E6,0)</f>
+        <v>427</v>
+      </c>
+      <c r="G6" s="3">
+        <f>F6/B2</f>
+        <v>17.791666666666668</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H9" si="13">(G6-C6)/C6</f>
+        <v>0.00078562843712451326</v>
+      </c>
+      <c r="J6" t="str">
+        <f>DEC2HEX(F6)</f>
+        <v>1AB</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="D7" s="4">
+        <f>B1/B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="11"/>
+        <v>37.333333333333336</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="12"/>
+        <v>37</v>
+      </c>
+      <c r="G7" s="5">
+        <f>F7/B2</f>
+        <v>1.5416666666666667</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="13"/>
+        <v>-0.008574490889603343</v>
+      </c>
+      <c r="J7" s="4" t="str">
+        <f>DEC2HEX(F7+F6)</f>
+        <v>1D0</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <f>B1/B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="11"/>
+        <v>37.333333333333336</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="12"/>
+        <v>37</v>
+      </c>
+      <c r="G8" s="5">
+        <f>F8/B2</f>
+        <v>1.5416666666666667</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="13"/>
+        <v>-0.008574490889603343</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" t="str">
+        <f>DEC2HEX(F6+F7+F8)</f>
+        <v>1F5</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.222</v>
+      </c>
+      <c r="D9" s="4">
+        <f>B1/B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="11"/>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="12"/>
+        <v>53</v>
+      </c>
+      <c r="G9" s="5">
+        <f>F9/B2</f>
+        <v>2.2083333333333335</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="13"/>
+        <v>-0.0061506150615060727</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" t="str">
+        <f>DEC2HEX(F6+F7+F8+F9)</f>
+        <v>22A</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <f>SUM(B6:B9)</f>
+        <v>832</v>
+      </c>
+      <c r="C10" s="3">
+        <v>23.109999999999999</v>
+      </c>
+      <c r="D10" s="4">
+        <f>B1/B2</f>
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="4">
+        <f>B10/D10</f>
+        <v>554.66666666666663</v>
+      </c>
+      <c r="F10" s="5">
+        <f>ROUND(E10,0)</f>
+        <v>555</v>
+      </c>
+      <c r="G10" s="5">
+        <f>F10/B2</f>
+        <v>23.125</v>
+      </c>
+      <c r="H10" s="6">
+        <f>(G10-C10)/C10</f>
+        <v>0.00064906966681092901</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>480</v>
+      </c>
+      <c r="C14">
+        <f>C10*B14/1000</f>
+        <v>11.092799999999999</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" ref="E14:E18" si="14">B14/D14</f>
+        <v>240</v>
+      </c>
+      <c r="F14" s="5">
+        <f>ROUND(E14,0)</f>
+        <v>240</v>
+      </c>
+      <c r="G14" s="3">
+        <f>F14/B2</f>
+        <v>10</v>
+      </c>
+      <c r="H14" s="6">
+        <f>(G14-C14)/C14</f>
+        <v>-0.098514351651521601</v>
+      </c>
+      <c r="J14" t="str">
+        <f>DEC2HEX(B14)</f>
+        <v>1E0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f>C10*B15/1000</f>
+        <v>0.023109999999999999</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" ref="F15:F17" si="15">E15</f>
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="5">
+        <f>F15/B2</f>
+        <v>0.020833333333333332</v>
+      </c>
+      <c r="H15" s="6">
+        <f>(G15-C15)*100/C15</f>
+        <v>-9.8514351651521697</v>
+      </c>
+      <c r="J15" t="str">
+        <f>DEC2HEX(B15+B14)</f>
+        <v>1E1</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f>C10*B16/1000</f>
+        <v>0.069330000000000003</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="14"/>
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="15"/>
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="5">
+        <f>F16/B2</f>
+        <v>0.0625</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" ref="H16:H18" si="16">(G16-C16)/C16</f>
+        <v>-0.098514351651521739</v>
+      </c>
+      <c r="J16" t="str">
+        <f>DEC2HEX(B16+B15+B14)</f>
+        <v>1E4</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <f>C10*B17/1000</f>
+        <v>0.57774999999999999</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="14"/>
+        <v>12.5</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="15"/>
+        <v>12.5</v>
+      </c>
+      <c r="G17" s="5">
+        <f>F17/B2</f>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="16"/>
+        <v>-0.098514351651521628</v>
+      </c>
+      <c r="J17" t="str">
+        <f>DEC2HEX(B14+B15+B16+B17)</f>
+        <v>1FD</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <f>SUM(B14:B17)</f>
+        <v>509</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C14:C17)</f>
+        <v>11.76299</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="14"/>
+        <v>254.5</v>
+      </c>
+      <c r="F18" s="5">
+        <f>SUM(F14:F17)</f>
+        <v>254.5</v>
+      </c>
+      <c r="G18" s="5">
+        <f>F18/B2</f>
+        <v>10.604166666666666</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="16"/>
+        <v>-0.098514351651521781</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25"/>
+    <row r="21" ht="14.25">
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s">
+        <v>48</v>
+      </c>
+      <c r="M21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="7">
+        <f>(C6*B14)/(C18*1000)</f>
+        <v>0.72543596483547124</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25"/>
+    <row r="25" ht="14.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <f>203*120</f>
+        <v>24360</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25"/>
+    <row r="27" ht="14.25"/>
+    <row r="28" ht="14.25"/>
+    <row r="30" ht="14.25"/>
+    <row r="32" ht="14.25"/>
+    <row r="33" ht="14.25">
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" ht="14.25"/>
+    <row r="35" ht="14.25">
+      <c r="D35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A12:E12"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="K1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="K3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
       <c r="W3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13">
+        <v>55</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+      <c r="M4" s="12">
         <v>2</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="12">
         <v>3</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="12">
         <v>4</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="12">
         <v>5</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="12">
         <v>6</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="12">
         <v>7</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="12">
         <v>8</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="12">
         <v>9</v>
       </c>
       <c r="U4" t="s">
-        <v>44</v>
-      </c>
-      <c r="W4" s="13">
-        <v>0</v>
-      </c>
-      <c r="X4" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="13">
+        <v>56</v>
+      </c>
+      <c r="W4" s="12">
+        <v>0</v>
+      </c>
+      <c r="X4" s="12">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="12">
         <v>2</v>
       </c>
-      <c r="Z4" s="13">
+      <c r="Z4" s="12">
         <v>3</v>
       </c>
-      <c r="AA4" s="13">
+      <c r="AA4" s="12">
         <v>4</v>
       </c>
-      <c r="AB4" s="13">
+      <c r="AB4" s="12">
         <v>5</v>
       </c>
-      <c r="AC4" s="13">
+      <c r="AC4" s="12">
         <v>6</v>
       </c>
-      <c r="AD4" s="13">
+      <c r="AD4" s="12">
         <v>7</v>
       </c>
-      <c r="AE4" s="13">
+      <c r="AE4" s="12">
         <v>8</v>
       </c>
-      <c r="AF4" s="13">
+      <c r="AF4" s="12">
         <v>9</v>
       </c>
       <c r="AG4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="I5">
-        <f>A5*(2^0)+B5*(2^1)+C5*(2^2)+D5*(2^3)+E5*(2^4)+F5*(2^5)+G5*(2^6)+H5*(2^7)</f>
+        <f t="shared" ref="I5:I9" si="17">A5*(2^0)+B5*(2^1)+C5*(2^2)+D5*(2^3)+E5*(2^4)+F5*(2^5)+G5*(2^6)+H5*(2^7)</f>
         <v>0</v>
       </c>
       <c r="K5">
@@ -1980,11 +3162,11 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <f>K5*(2^0)+L5*(2^1)+M5*(2^2)+N5*(2^3)+O5*(2^4)+P5*(2^5)+Q5*(2^6)+R5*(2^7)+S5*(2^8)+T5*(2^9)</f>
+        <f t="shared" ref="U5:U9" si="18">K5*(2^0)+L5*(2^1)+M5*(2^2)+N5*(2^3)+O5*(2^4)+P5*(2^5)+Q5*(2^6)+R5*(2^7)+S5*(2^8)+T5*(2^9)</f>
         <v>0</v>
       </c>
       <c r="W5" s="4">
-        <f>I5+_xlfn.BITLSHIFT(U5,8)</f>
+        <f t="shared" ref="W5:W9" si="19">I5+_xlfn.BITLSHIFT(U5,8)</f>
         <v>0</v>
       </c>
       <c r="X5" s="4">
@@ -2015,17 +3197,17 @@
         <v>0</v>
       </c>
       <c r="AG5" s="4">
-        <f>W5*(2^0)+X5*(2^1)+Y5*(2^2)+Z5*(2^3)+AA5*(2^4)+AB5*(2^5)+AC5*(2^6)+AD5*(2^7)+AE5*(2^8)+AF5*(2^9)</f>
+        <f t="shared" ref="AG5:AG8" si="20">W5*(2^0)+X5*(2^1)+Y5*(2^2)+Z5*(2^3)+AA5*(2^4)+AB5*(2^5)+AC5*(2^6)+AD5*(2^7)+AE5*(2^8)+AF5*(2^9)</f>
         <v>0</v>
       </c>
       <c r="AI5">
-        <f>U5+_xlfn.BITLSHIFT(AG5,7)</f>
+        <f t="shared" ref="AI5:AI9" si="21">U5+_xlfn.BITLSHIFT(AG5,7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="I6">
-        <f>A6*(2^0)+B6*(2^1)+C6*(2^2)+D6*(2^3)+E6*(2^4)+F6*(2^5)+G6*(2^6)+H6*(2^7)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K6" s="4">
@@ -2059,11 +3241,11 @@
         <v>0</v>
       </c>
       <c r="U6" s="4">
-        <f>K6*(2^0)+L6*(2^1)+M6*(2^2)+N6*(2^3)+O6*(2^4)+P6*(2^5)+Q6*(2^6)+R6*(2^7)+S6*(2^8)+T6*(2^9)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W6">
-        <f>I6+_xlfn.BITLSHIFT(U6,8)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X6" s="4">
@@ -2094,17 +3276,17 @@
         <v>0</v>
       </c>
       <c r="AG6" s="4">
-        <f>W6*(2^0)+X6*(2^1)+Y6*(2^2)+Z6*(2^3)+AA6*(2^4)+AB6*(2^5)+AC6*(2^6)+AD6*(2^7)+AE6*(2^8)+AF6*(2^9)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AI6" s="4">
-        <f>U6+_xlfn.BITLSHIFT(AG6,7)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="I7">
-        <f>A7*(2^0)+B7*(2^1)+C7*(2^2)+D7*(2^3)+E7*(2^4)+F7*(2^5)+G7*(2^6)+H7*(2^7)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K7" s="4">
@@ -2138,11 +3320,11 @@
         <v>0</v>
       </c>
       <c r="U7" s="4">
-        <f>K7*(2^0)+L7*(2^1)+M7*(2^2)+N7*(2^3)+O7*(2^4)+P7*(2^5)+Q7*(2^6)+R7*(2^7)+S7*(2^8)+T7*(2^9)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W7">
-        <f>I7+_xlfn.BITLSHIFT(U7,8)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X7" s="4">
@@ -2173,17 +3355,17 @@
         <v>0</v>
       </c>
       <c r="AG7" s="4">
-        <f>W7*(2^0)+X7*(2^1)+Y7*(2^2)+Z7*(2^3)+AA7*(2^4)+AB7*(2^5)+AC7*(2^6)+AD7*(2^7)+AE7*(2^8)+AF7*(2^9)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="AI7" s="4">
-        <f>U7+_xlfn.BITLSHIFT(AG7,7)</f>
+        <f t="shared" si="21"/>
         <v>256</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="I8">
-        <f>A8*(2^0)+B8*(2^1)+C8*(2^2)+D8*(2^3)+E8*(2^4)+F8*(2^5)+G8*(2^6)+H8*(2^7)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="K8" s="4">
@@ -2217,11 +3399,11 @@
         <v>0</v>
       </c>
       <c r="U8" s="4">
-        <f>K8*(2^0)+L8*(2^1)+M8*(2^2)+N8*(2^3)+O8*(2^4)+P8*(2^5)+Q8*(2^6)+R8*(2^7)+S8*(2^8)+T8*(2^9)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W8">
-        <f>I8+_xlfn.BITLSHIFT(U8,8)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X8" s="4">
@@ -2252,11 +3434,11 @@
         <v>0</v>
       </c>
       <c r="AG8" s="4">
-        <f>W8*(2^0)+X8*(2^1)+Y8*(2^2)+Z8*(2^3)+AA8*(2^4)+AB8*(2^5)+AC8*(2^6)+AD8*(2^7)+AE8*(2^8)+AF8*(2^9)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="AI8" s="4">
-        <f>U8+_xlfn.BITLSHIFT(AG8,7)</f>
+        <f t="shared" si="21"/>
         <v>256</v>
       </c>
     </row>
@@ -2271,7 +3453,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <f>A9*(2^0)+B9*(2^1)+C9*(2^2)+D9*(2^3)+E9*(2^4)+F9*(2^5)+G9*(2^6)+H9*(2^7)</f>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="K9" s="4">
@@ -2305,15 +3487,15 @@
         <v>0</v>
       </c>
       <c r="U9" s="4">
-        <f>K9*(2^0)+L9*(2^1)+M9*(2^2)+N9*(2^3)+O9*(2^4)+P9*(2^5)+Q9*(2^6)+R9*(2^7)+S9*(2^8)+T9*(2^9)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="W9">
-        <f>I9+_xlfn.BITLSHIFT(U9,8)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="AI9" s="4">
-        <f>U9+_xlfn.BITLSHIFT(AG9,7)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -2328,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <f>A10*(2^0)+B10*(2^1)+C10*(2^2)+D10*(2^3)+E10*(2^4)+F10*(2^5)+G10*(2^6)+H10*(2^7)</f>
+        <f t="shared" ref="I10:I58" si="22">A10*(2^0)+B10*(2^1)+C10*(2^2)+D10*(2^3)+E10*(2^4)+F10*(2^5)+G10*(2^6)+H10*(2^7)</f>
         <v>5</v>
       </c>
       <c r="K10" s="4">
@@ -2362,15 +3544,15 @@
         <v>0</v>
       </c>
       <c r="U10" s="4">
-        <f>K10*(2^0)+L10*(2^1)+M10*(2^2)+N10*(2^3)+O10*(2^4)+P10*(2^5)+Q10*(2^6)+R10*(2^7)+S10*(2^8)+T10*(2^9)</f>
+        <f t="shared" ref="U10:U58" si="23">K10*(2^0)+L10*(2^1)+M10*(2^2)+N10*(2^3)+O10*(2^4)+P10*(2^5)+Q10*(2^6)+R10*(2^7)+S10*(2^8)+T10*(2^9)</f>
         <v>0</v>
       </c>
       <c r="W10">
-        <f>I10+_xlfn.BITLSHIFT(U10,8)</f>
+        <f t="shared" ref="W10:W58" si="24">I10+_xlfn.BITLSHIFT(U10,8)</f>
         <v>5</v>
       </c>
       <c r="AI10" s="4">
-        <f>U10+_xlfn.BITLSHIFT(AG10,7)</f>
+        <f t="shared" ref="AI10:AI12" si="25">U10+_xlfn.BITLSHIFT(AG10,7)</f>
         <v>0</v>
       </c>
     </row>
@@ -2385,7 +3567,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <f>A11*(2^0)+B11*(2^1)+C11*(2^2)+D11*(2^3)+E11*(2^4)+F11*(2^5)+G11*(2^6)+H11*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
       <c r="K11" s="4">
@@ -2419,15 +3601,15 @@
         <v>0</v>
       </c>
       <c r="U11" s="4">
-        <f>K11*(2^0)+L11*(2^1)+M11*(2^2)+N11*(2^3)+O11*(2^4)+P11*(2^5)+Q11*(2^6)+R11*(2^7)+S11*(2^8)+T11*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W11">
-        <f>I11+_xlfn.BITLSHIFT(U11,8)</f>
+        <f t="shared" si="24"/>
         <v>6</v>
       </c>
       <c r="AI11" s="4">
-        <f>U11+_xlfn.BITLSHIFT(AG11,7)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -2442,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <f>A12*(2^0)+B12*(2^1)+C12*(2^2)+D12*(2^3)+E12*(2^4)+F12*(2^5)+G12*(2^6)+H12*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="K12" s="4">
@@ -2476,15 +3658,15 @@
         <v>0</v>
       </c>
       <c r="U12" s="4">
-        <f>K12*(2^0)+L12*(2^1)+M12*(2^2)+N12*(2^3)+O12*(2^4)+P12*(2^5)+Q12*(2^6)+R12*(2^7)+S12*(2^8)+T12*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W12">
-        <f>I12+_xlfn.BITLSHIFT(U12,8)</f>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="AI12" s="4">
-        <f>U12+_xlfn.BITLSHIFT(AG12,7)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -2502,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <f>A13*(2^0)+B13*(2^1)+C13*(2^2)+D13*(2^3)+E13*(2^4)+F13*(2^5)+G13*(2^6)+H13*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="K13" s="4">
@@ -2536,11 +3718,11 @@
         <v>0</v>
       </c>
       <c r="U13" s="4">
-        <f>K13*(2^0)+L13*(2^1)+M13*(2^2)+N13*(2^3)+O13*(2^4)+P13*(2^5)+Q13*(2^6)+R13*(2^7)+S13*(2^8)+T13*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f>I13+_xlfn.BITLSHIFT(U13,8)</f>
+        <f t="shared" si="24"/>
         <v>8</v>
       </c>
     </row>
@@ -2570,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <f>A14*(2^0)+B14*(2^1)+C14*(2^2)+D14*(2^3)+E14*(2^4)+F14*(2^5)+G14*(2^6)+H14*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>211</v>
       </c>
       <c r="K14" s="4">
@@ -2604,11 +3786,11 @@
         <v>0</v>
       </c>
       <c r="U14" s="4">
-        <f>K14*(2^0)+L14*(2^1)+M14*(2^2)+N14*(2^3)+O14*(2^4)+P14*(2^5)+Q14*(2^6)+R14*(2^7)+S14*(2^8)+T14*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f>I14+_xlfn.BITLSHIFT(U14,8)</f>
+        <f t="shared" si="24"/>
         <v>211</v>
       </c>
     </row>
@@ -2649,18 +3831,18 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f>A16*(2^0)+B16*(2^1)+C16*(2^2)+D16*(2^3)+E16*(2^4)+F16*(2^5)+G16*(2^6)+H16*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="U16" s="4">
-        <f>K16*(2^0)+L16*(2^1)+M16*(2^2)+N16*(2^3)+O16*(2^4)+P16*(2^5)+Q16*(2^6)+R16*(2^7)+S16*(2^8)+T16*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W16">
-        <f>I16+_xlfn.BITLSHIFT(U16,8)</f>
+        <f t="shared" si="24"/>
         <v>256</v>
       </c>
     </row>
@@ -2690,18 +3872,18 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <f>A17*(2^0)+B17*(2^1)+C17*(2^2)+D17*(2^3)+E17*(2^4)+F17*(2^5)+G17*(2^6)+H17*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="U17" s="4">
-        <f>K17*(2^0)+L17*(2^1)+M17*(2^2)+N17*(2^3)+O17*(2^4)+P17*(2^5)+Q17*(2^6)+R17*(2^7)+S17*(2^8)+T17*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W17">
-        <f>I17+_xlfn.BITLSHIFT(U17,8)</f>
+        <f t="shared" si="24"/>
         <v>257</v>
       </c>
     </row>
@@ -2731,18 +3913,18 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <f>A18*(2^0)+B18*(2^1)+C18*(2^2)+D18*(2^3)+E18*(2^4)+F18*(2^5)+G18*(2^6)+H18*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="U18" s="4">
-        <f>K18*(2^0)+L18*(2^1)+M18*(2^2)+N18*(2^3)+O18*(2^4)+P18*(2^5)+Q18*(2^6)+R18*(2^7)+S18*(2^8)+T18*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W18">
-        <f>I18+_xlfn.BITLSHIFT(U18,8)</f>
+        <f t="shared" si="24"/>
         <v>258</v>
       </c>
     </row>
@@ -2772,18 +3954,18 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <f>A19*(2^0)+B19*(2^1)+C19*(2^2)+D19*(2^3)+E19*(2^4)+F19*(2^5)+G19*(2^6)+H19*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="U19" s="4">
-        <f>K19*(2^0)+L19*(2^1)+M19*(2^2)+N19*(2^3)+O19*(2^4)+P19*(2^5)+Q19*(2^6)+R19*(2^7)+S19*(2^8)+T19*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W19">
-        <f>I19+_xlfn.BITLSHIFT(U19,8)</f>
+        <f t="shared" si="24"/>
         <v>259</v>
       </c>
     </row>
@@ -2803,18 +3985,18 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20">
-        <f>A20*(2^0)+B20*(2^1)+C20*(2^2)+D20*(2^3)+E20*(2^4)+F20*(2^5)+G20*(2^6)+H20*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="U20" s="4">
-        <f>K20*(2^0)+L20*(2^1)+M20*(2^2)+N20*(2^3)+O20*(2^4)+P20*(2^5)+Q20*(2^6)+R20*(2^7)+S20*(2^8)+T20*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W20">
-        <f>I20+_xlfn.BITLSHIFT(U20,8)</f>
+        <f t="shared" si="24"/>
         <v>260</v>
       </c>
     </row>
@@ -2834,18 +4016,18 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21">
-        <f>A21*(2^0)+B21*(2^1)+C21*(2^2)+D21*(2^3)+E21*(2^4)+F21*(2^5)+G21*(2^6)+H21*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="U21" s="4">
-        <f>K21*(2^0)+L21*(2^1)+M21*(2^2)+N21*(2^3)+O21*(2^4)+P21*(2^5)+Q21*(2^6)+R21*(2^7)+S21*(2^8)+T21*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W21">
-        <f>I21+_xlfn.BITLSHIFT(U21,8)</f>
+        <f t="shared" si="24"/>
         <v>261</v>
       </c>
     </row>
@@ -2865,18 +4047,18 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22">
-        <f>A22*(2^0)+B22*(2^1)+C22*(2^2)+D22*(2^3)+E22*(2^4)+F22*(2^5)+G22*(2^6)+H22*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
       <c r="U22" s="4">
-        <f>K22*(2^0)+L22*(2^1)+M22*(2^2)+N22*(2^3)+O22*(2^4)+P22*(2^5)+Q22*(2^6)+R22*(2^7)+S22*(2^8)+T22*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W22">
-        <f>I22+_xlfn.BITLSHIFT(U22,8)</f>
+        <f t="shared" si="24"/>
         <v>262</v>
       </c>
     </row>
@@ -2896,18 +4078,18 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23">
-        <f>A23*(2^0)+B23*(2^1)+C23*(2^2)+D23*(2^3)+E23*(2^4)+F23*(2^5)+G23*(2^6)+H23*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="U23" s="4">
-        <f>K23*(2^0)+L23*(2^1)+M23*(2^2)+N23*(2^3)+O23*(2^4)+P23*(2^5)+Q23*(2^6)+R23*(2^7)+S23*(2^8)+T23*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W23">
-        <f>I23+_xlfn.BITLSHIFT(U23,8)</f>
+        <f t="shared" si="24"/>
         <v>263</v>
       </c>
     </row>
@@ -2929,18 +4111,18 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24">
-        <f>A24*(2^0)+B24*(2^1)+C24*(2^2)+D24*(2^3)+E24*(2^4)+F24*(2^5)+G24*(2^6)+H24*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="U24" s="4">
-        <f>K24*(2^0)+L24*(2^1)+M24*(2^2)+N24*(2^3)+O24*(2^4)+P24*(2^5)+Q24*(2^6)+R24*(2^7)+S24*(2^8)+T24*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W24">
-        <f>I24+_xlfn.BITLSHIFT(U24,8)</f>
+        <f t="shared" si="24"/>
         <v>264</v>
       </c>
     </row>
@@ -2970,18 +4152,18 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f>A25*(2^0)+B25*(2^1)+C25*(2^2)+D25*(2^3)+E25*(2^4)+F25*(2^5)+G25*(2^6)+H25*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>211</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
       <c r="U25" s="4">
-        <f>K25*(2^0)+L25*(2^1)+M25*(2^2)+N25*(2^3)+O25*(2^4)+P25*(2^5)+Q25*(2^6)+R25*(2^7)+S25*(2^8)+T25*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="W25">
-        <f>I25+_xlfn.BITLSHIFT(U25,8)</f>
+        <f t="shared" si="24"/>
         <v>467</v>
       </c>
     </row>
@@ -3014,18 +4196,18 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f>A27*(2^0)+B27*(2^1)+C27*(2^2)+D27*(2^3)+E27*(2^4)+F27*(2^5)+G27*(2^6)+H27*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L27">
         <v>1</v>
       </c>
       <c r="U27" s="4">
-        <f>K27*(2^0)+L27*(2^1)+M27*(2^2)+N27*(2^3)+O27*(2^4)+P27*(2^5)+Q27*(2^6)+R27*(2^7)+S27*(2^8)+T27*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W27">
-        <f>I27+_xlfn.BITLSHIFT(U27,8)</f>
+        <f t="shared" si="24"/>
         <v>512</v>
       </c>
     </row>
@@ -3055,18 +4237,18 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <f>A28*(2^0)+B28*(2^1)+C28*(2^2)+D28*(2^3)+E28*(2^4)+F28*(2^5)+G28*(2^6)+H28*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="L28" s="4">
         <v>1</v>
       </c>
       <c r="U28" s="4">
-        <f>K28*(2^0)+L28*(2^1)+M28*(2^2)+N28*(2^3)+O28*(2^4)+P28*(2^5)+Q28*(2^6)+R28*(2^7)+S28*(2^8)+T28*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W28">
-        <f>I28+_xlfn.BITLSHIFT(U28,8)</f>
+        <f t="shared" si="24"/>
         <v>513</v>
       </c>
     </row>
@@ -3096,18 +4278,18 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <f>A29*(2^0)+B29*(2^1)+C29*(2^2)+D29*(2^3)+E29*(2^4)+F29*(2^5)+G29*(2^6)+H29*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="L29" s="4">
         <v>1</v>
       </c>
       <c r="U29" s="4">
-        <f>K29*(2^0)+L29*(2^1)+M29*(2^2)+N29*(2^3)+O29*(2^4)+P29*(2^5)+Q29*(2^6)+R29*(2^7)+S29*(2^8)+T29*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W29">
-        <f>I29+_xlfn.BITLSHIFT(U29,8)</f>
+        <f t="shared" si="24"/>
         <v>514</v>
       </c>
     </row>
@@ -3137,18 +4319,18 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <f>A30*(2^0)+B30*(2^1)+C30*(2^2)+D30*(2^3)+E30*(2^4)+F30*(2^5)+G30*(2^6)+H30*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
       <c r="L30" s="4">
         <v>1</v>
       </c>
       <c r="U30" s="4">
-        <f>K30*(2^0)+L30*(2^1)+M30*(2^2)+N30*(2^3)+O30*(2^4)+P30*(2^5)+Q30*(2^6)+R30*(2^7)+S30*(2^8)+T30*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W30">
-        <f>I30+_xlfn.BITLSHIFT(U30,8)</f>
+        <f t="shared" si="24"/>
         <v>515</v>
       </c>
     </row>
@@ -3168,18 +4350,18 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31">
-        <f>A31*(2^0)+B31*(2^1)+C31*(2^2)+D31*(2^3)+E31*(2^4)+F31*(2^5)+G31*(2^6)+H31*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="L31" s="4">
         <v>1</v>
       </c>
       <c r="U31" s="4">
-        <f>K31*(2^0)+L31*(2^1)+M31*(2^2)+N31*(2^3)+O31*(2^4)+P31*(2^5)+Q31*(2^6)+R31*(2^7)+S31*(2^8)+T31*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W31">
-        <f>I31+_xlfn.BITLSHIFT(U31,8)</f>
+        <f t="shared" si="24"/>
         <v>516</v>
       </c>
     </row>
@@ -3199,18 +4381,18 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32">
-        <f>A32*(2^0)+B32*(2^1)+C32*(2^2)+D32*(2^3)+E32*(2^4)+F32*(2^5)+G32*(2^6)+H32*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="L32" s="4">
         <v>1</v>
       </c>
       <c r="U32" s="4">
-        <f>K32*(2^0)+L32*(2^1)+M32*(2^2)+N32*(2^3)+O32*(2^4)+P32*(2^5)+Q32*(2^6)+R32*(2^7)+S32*(2^8)+T32*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W32">
-        <f>I32+_xlfn.BITLSHIFT(U32,8)</f>
+        <f t="shared" si="24"/>
         <v>517</v>
       </c>
     </row>
@@ -3230,18 +4412,18 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33">
-        <f>A33*(2^0)+B33*(2^1)+C33*(2^2)+D33*(2^3)+E33*(2^4)+F33*(2^5)+G33*(2^6)+H33*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
       <c r="L33" s="4">
         <v>1</v>
       </c>
       <c r="U33" s="4">
-        <f>K33*(2^0)+L33*(2^1)+M33*(2^2)+N33*(2^3)+O33*(2^4)+P33*(2^5)+Q33*(2^6)+R33*(2^7)+S33*(2^8)+T33*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W33">
-        <f>I33+_xlfn.BITLSHIFT(U33,8)</f>
+        <f t="shared" si="24"/>
         <v>518</v>
       </c>
     </row>
@@ -3261,18 +4443,18 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34">
-        <f>A34*(2^0)+B34*(2^1)+C34*(2^2)+D34*(2^3)+E34*(2^4)+F34*(2^5)+G34*(2^6)+H34*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="L34" s="4">
         <v>1</v>
       </c>
       <c r="U34" s="4">
-        <f>K34*(2^0)+L34*(2^1)+M34*(2^2)+N34*(2^3)+O34*(2^4)+P34*(2^5)+Q34*(2^6)+R34*(2^7)+S34*(2^8)+T34*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W34">
-        <f>I34+_xlfn.BITLSHIFT(U34,8)</f>
+        <f t="shared" si="24"/>
         <v>519</v>
       </c>
     </row>
@@ -3294,18 +4476,18 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35">
-        <f>A35*(2^0)+B35*(2^1)+C35*(2^2)+D35*(2^3)+E35*(2^4)+F35*(2^5)+G35*(2^6)+H35*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="U35" s="4">
-        <f>K35*(2^0)+L35*(2^1)+M35*(2^2)+N35*(2^3)+O35*(2^4)+P35*(2^5)+Q35*(2^6)+R35*(2^7)+S35*(2^8)+T35*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W35">
-        <f>I35+_xlfn.BITLSHIFT(U35,8)</f>
+        <f t="shared" si="24"/>
         <v>520</v>
       </c>
     </row>
@@ -3335,18 +4517,18 @@
         <v>1</v>
       </c>
       <c r="I36">
-        <f>A36*(2^0)+B36*(2^1)+C36*(2^2)+D36*(2^3)+E36*(2^4)+F36*(2^5)+G36*(2^6)+H36*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>211</v>
       </c>
       <c r="L36" s="4">
         <v>1</v>
       </c>
       <c r="U36" s="4">
-        <f>K36*(2^0)+L36*(2^1)+M36*(2^2)+N36*(2^3)+O36*(2^4)+P36*(2^5)+Q36*(2^6)+R36*(2^7)+S36*(2^8)+T36*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="W36">
-        <f>I36+_xlfn.BITLSHIFT(U36,8)</f>
+        <f t="shared" si="24"/>
         <v>723</v>
       </c>
     </row>
@@ -3379,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="4">
-        <f>A38*(2^0)+B38*(2^1)+C38*(2^2)+D38*(2^3)+E38*(2^4)+F38*(2^5)+G38*(2^6)+H38*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J38" s="4"/>
@@ -3398,12 +4580,12 @@
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4">
-        <f>K38*(2^0)+L38*(2^1)+M38*(2^2)+N38*(2^3)+O38*(2^4)+P38*(2^5)+Q38*(2^6)+R38*(2^7)+S38*(2^8)+T38*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V38" s="4"/>
       <c r="W38" s="4">
-        <f>I38+_xlfn.BITLSHIFT(U38,8)</f>
+        <f t="shared" si="24"/>
         <v>768</v>
       </c>
     </row>
@@ -3433,7 +4615,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="4">
-        <f>A39*(2^0)+B39*(2^1)+C39*(2^2)+D39*(2^3)+E39*(2^4)+F39*(2^5)+G39*(2^6)+H39*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="J39" s="4"/>
@@ -3452,12 +4634,12 @@
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
       <c r="U39" s="4">
-        <f>K39*(2^0)+L39*(2^1)+M39*(2^2)+N39*(2^3)+O39*(2^4)+P39*(2^5)+Q39*(2^6)+R39*(2^7)+S39*(2^8)+T39*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V39" s="4"/>
       <c r="W39" s="4">
-        <f>I39+_xlfn.BITLSHIFT(U39,8)</f>
+        <f t="shared" si="24"/>
         <v>769</v>
       </c>
     </row>
@@ -3487,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="4">
-        <f>A40*(2^0)+B40*(2^1)+C40*(2^2)+D40*(2^3)+E40*(2^4)+F40*(2^5)+G40*(2^6)+H40*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="J40" s="4"/>
@@ -3506,12 +4688,12 @@
       <c r="S40" s="4"/>
       <c r="T40" s="4"/>
       <c r="U40" s="4">
-        <f>K40*(2^0)+L40*(2^1)+M40*(2^2)+N40*(2^3)+O40*(2^4)+P40*(2^5)+Q40*(2^6)+R40*(2^7)+S40*(2^8)+T40*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V40" s="4"/>
       <c r="W40" s="4">
-        <f>I40+_xlfn.BITLSHIFT(U40,8)</f>
+        <f t="shared" si="24"/>
         <v>770</v>
       </c>
     </row>
@@ -3541,7 +4723,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="4">
-        <f>A41*(2^0)+B41*(2^1)+C41*(2^2)+D41*(2^3)+E41*(2^4)+F41*(2^5)+G41*(2^6)+H41*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
       <c r="J41" s="4"/>
@@ -3560,12 +4742,12 @@
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
       <c r="U41" s="4">
-        <f>K41*(2^0)+L41*(2^1)+M41*(2^2)+N41*(2^3)+O41*(2^4)+P41*(2^5)+Q41*(2^6)+R41*(2^7)+S41*(2^8)+T41*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V41" s="4"/>
       <c r="W41" s="4">
-        <f>I41+_xlfn.BITLSHIFT(U41,8)</f>
+        <f t="shared" si="24"/>
         <v>771</v>
       </c>
     </row>
@@ -3585,7 +4767,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4">
-        <f>A42*(2^0)+B42*(2^1)+C42*(2^2)+D42*(2^3)+E42*(2^4)+F42*(2^5)+G42*(2^6)+H42*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="J42" s="4"/>
@@ -3604,12 +4786,12 @@
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
       <c r="U42" s="4">
-        <f>K42*(2^0)+L42*(2^1)+M42*(2^2)+N42*(2^3)+O42*(2^4)+P42*(2^5)+Q42*(2^6)+R42*(2^7)+S42*(2^8)+T42*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V42" s="4"/>
       <c r="W42" s="4">
-        <f>I42+_xlfn.BITLSHIFT(U42,8)</f>
+        <f t="shared" si="24"/>
         <v>772</v>
       </c>
     </row>
@@ -3629,7 +4811,7 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4">
-        <f>A43*(2^0)+B43*(2^1)+C43*(2^2)+D43*(2^3)+E43*(2^4)+F43*(2^5)+G43*(2^6)+H43*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="J43" s="4"/>
@@ -3648,12 +4830,12 @@
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
       <c r="U43" s="4">
-        <f>K43*(2^0)+L43*(2^1)+M43*(2^2)+N43*(2^3)+O43*(2^4)+P43*(2^5)+Q43*(2^6)+R43*(2^7)+S43*(2^8)+T43*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V43" s="4"/>
       <c r="W43" s="4">
-        <f>I43+_xlfn.BITLSHIFT(U43,8)</f>
+        <f t="shared" si="24"/>
         <v>773</v>
       </c>
     </row>
@@ -3673,7 +4855,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4">
-        <f>A44*(2^0)+B44*(2^1)+C44*(2^2)+D44*(2^3)+E44*(2^4)+F44*(2^5)+G44*(2^6)+H44*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
       <c r="J44" s="4"/>
@@ -3692,12 +4874,12 @@
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
       <c r="U44" s="4">
-        <f>K44*(2^0)+L44*(2^1)+M44*(2^2)+N44*(2^3)+O44*(2^4)+P44*(2^5)+Q44*(2^6)+R44*(2^7)+S44*(2^8)+T44*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V44" s="4"/>
       <c r="W44" s="4">
-        <f>I44+_xlfn.BITLSHIFT(U44,8)</f>
+        <f t="shared" si="24"/>
         <v>774</v>
       </c>
     </row>
@@ -3717,7 +4899,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4">
-        <f>A45*(2^0)+B45*(2^1)+C45*(2^2)+D45*(2^3)+E45*(2^4)+F45*(2^5)+G45*(2^6)+H45*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="J45" s="4"/>
@@ -3736,12 +4918,12 @@
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
       <c r="U45" s="4">
-        <f>K45*(2^0)+L45*(2^1)+M45*(2^2)+N45*(2^3)+O45*(2^4)+P45*(2^5)+Q45*(2^6)+R45*(2^7)+S45*(2^8)+T45*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V45" s="4"/>
       <c r="W45" s="4">
-        <f>I45+_xlfn.BITLSHIFT(U45,8)</f>
+        <f t="shared" si="24"/>
         <v>775</v>
       </c>
     </row>
@@ -3763,7 +4945,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4">
-        <f>A46*(2^0)+B46*(2^1)+C46*(2^2)+D46*(2^3)+E46*(2^4)+F46*(2^5)+G46*(2^6)+H46*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="J46" s="4"/>
@@ -3782,12 +4964,12 @@
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
       <c r="U46" s="4">
-        <f>K46*(2^0)+L46*(2^1)+M46*(2^2)+N46*(2^3)+O46*(2^4)+P46*(2^5)+Q46*(2^6)+R46*(2^7)+S46*(2^8)+T46*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V46" s="4"/>
       <c r="W46" s="4">
-        <f>I46+_xlfn.BITLSHIFT(U46,8)</f>
+        <f t="shared" si="24"/>
         <v>776</v>
       </c>
     </row>
@@ -3817,7 +4999,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="4">
-        <f>A47*(2^0)+B47*(2^1)+C47*(2^2)+D47*(2^3)+E47*(2^4)+F47*(2^5)+G47*(2^6)+H47*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>211</v>
       </c>
       <c r="J47" s="4"/>
@@ -3836,41 +5018,41 @@
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
       <c r="U47" s="4">
-        <f>K47*(2^0)+L47*(2^1)+M47*(2^2)+N47*(2^3)+O47*(2^4)+P47*(2^5)+Q47*(2^6)+R47*(2^7)+S47*(2^8)+T47*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="V47" s="4"/>
       <c r="W47" s="4">
-        <f>I47+_xlfn.BITLSHIFT(U47,8)</f>
+        <f t="shared" si="24"/>
         <v>979</v>
       </c>
     </row>
     <row r="48" ht="14.25">
-      <c r="A48" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
+      <c r="A48" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="13"/>
     </row>
     <row r="49" ht="14.25">
       <c r="A49" s="4">
@@ -3898,7 +5080,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="4">
-        <f>A49*(2^0)+B49*(2^1)+C49*(2^2)+D49*(2^3)+E49*(2^4)+F49*(2^5)+G49*(2^6)+H49*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J49" s="4"/>
@@ -3933,12 +5115,12 @@
         <v>1</v>
       </c>
       <c r="U49" s="4">
-        <f>K49*(2^0)+L49*(2^1)+M49*(2^2)+N49*(2^3)+O49*(2^4)+P49*(2^5)+Q49*(2^6)+R49*(2^7)+S49*(2^8)+T49*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V49" s="4"/>
       <c r="W49" s="4">
-        <f>I49+_xlfn.BITLSHIFT(U49,8)</f>
+        <f t="shared" si="24"/>
         <v>160768</v>
       </c>
     </row>
@@ -3968,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="4">
-        <f>A50*(2^0)+B50*(2^1)+C50*(2^2)+D50*(2^3)+E50*(2^4)+F50*(2^5)+G50*(2^6)+H50*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="J50" s="4"/>
@@ -4003,12 +5185,12 @@
         <v>1</v>
       </c>
       <c r="U50" s="4">
-        <f>K50*(2^0)+L50*(2^1)+M50*(2^2)+N50*(2^3)+O50*(2^4)+P50*(2^5)+Q50*(2^6)+R50*(2^7)+S50*(2^8)+T50*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V50" s="4"/>
       <c r="W50" s="4">
-        <f>I50+_xlfn.BITLSHIFT(U50,8)</f>
+        <f t="shared" si="24"/>
         <v>160769</v>
       </c>
     </row>
@@ -4038,7 +5220,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="4">
-        <f>A51*(2^0)+B51*(2^1)+C51*(2^2)+D51*(2^3)+E51*(2^4)+F51*(2^5)+G51*(2^6)+H51*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="J51" s="4"/>
@@ -4073,12 +5255,12 @@
         <v>1</v>
       </c>
       <c r="U51" s="4">
-        <f>K51*(2^0)+L51*(2^1)+M51*(2^2)+N51*(2^3)+O51*(2^4)+P51*(2^5)+Q51*(2^6)+R51*(2^7)+S51*(2^8)+T51*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V51" s="4"/>
       <c r="W51" s="4">
-        <f>I51+_xlfn.BITLSHIFT(U51,8)</f>
+        <f t="shared" si="24"/>
         <v>160770</v>
       </c>
     </row>
@@ -4108,7 +5290,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="4">
-        <f>A52*(2^0)+B52*(2^1)+C52*(2^2)+D52*(2^3)+E52*(2^4)+F52*(2^5)+G52*(2^6)+H52*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
       <c r="J52" s="4"/>
@@ -4143,12 +5325,12 @@
         <v>1</v>
       </c>
       <c r="U52" s="4">
-        <f>K52*(2^0)+L52*(2^1)+M52*(2^2)+N52*(2^3)+O52*(2^4)+P52*(2^5)+Q52*(2^6)+R52*(2^7)+S52*(2^8)+T52*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V52" s="4"/>
       <c r="W52" s="4">
-        <f>I52+_xlfn.BITLSHIFT(U52,8)</f>
+        <f t="shared" si="24"/>
         <v>160771</v>
       </c>
     </row>
@@ -4168,7 +5350,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4">
-        <f>A53*(2^0)+B53*(2^1)+C53*(2^2)+D53*(2^3)+E53*(2^4)+F53*(2^5)+G53*(2^6)+H53*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>4</v>
       </c>
       <c r="J53" s="4"/>
@@ -4203,12 +5385,12 @@
         <v>1</v>
       </c>
       <c r="U53" s="4">
-        <f>K53*(2^0)+L53*(2^1)+M53*(2^2)+N53*(2^3)+O53*(2^4)+P53*(2^5)+Q53*(2^6)+R53*(2^7)+S53*(2^8)+T53*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V53" s="4"/>
       <c r="W53" s="4">
-        <f>I53+_xlfn.BITLSHIFT(U53,8)</f>
+        <f t="shared" si="24"/>
         <v>160772</v>
       </c>
     </row>
@@ -4228,7 +5410,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4">
-        <f>A54*(2^0)+B54*(2^1)+C54*(2^2)+D54*(2^3)+E54*(2^4)+F54*(2^5)+G54*(2^6)+H54*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="J54" s="4"/>
@@ -4263,12 +5445,12 @@
         <v>1</v>
       </c>
       <c r="U54" s="4">
-        <f>K54*(2^0)+L54*(2^1)+M54*(2^2)+N54*(2^3)+O54*(2^4)+P54*(2^5)+Q54*(2^6)+R54*(2^7)+S54*(2^8)+T54*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V54" s="4"/>
       <c r="W54" s="4">
-        <f>I54+_xlfn.BITLSHIFT(U54,8)</f>
+        <f t="shared" si="24"/>
         <v>160773</v>
       </c>
     </row>
@@ -4288,7 +5470,7 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4">
-        <f>A55*(2^0)+B55*(2^1)+C55*(2^2)+D55*(2^3)+E55*(2^4)+F55*(2^5)+G55*(2^6)+H55*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>6</v>
       </c>
       <c r="J55" s="4"/>
@@ -4323,12 +5505,12 @@
         <v>1</v>
       </c>
       <c r="U55" s="4">
-        <f>K55*(2^0)+L55*(2^1)+M55*(2^2)+N55*(2^3)+O55*(2^4)+P55*(2^5)+Q55*(2^6)+R55*(2^7)+S55*(2^8)+T55*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V55" s="4"/>
       <c r="W55" s="4">
-        <f>I55+_xlfn.BITLSHIFT(U55,8)</f>
+        <f t="shared" si="24"/>
         <v>160774</v>
       </c>
     </row>
@@ -4348,7 +5530,7 @@
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4">
-        <f>A56*(2^0)+B56*(2^1)+C56*(2^2)+D56*(2^3)+E56*(2^4)+F56*(2^5)+G56*(2^6)+H56*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="J56" s="4"/>
@@ -4383,12 +5565,12 @@
         <v>1</v>
       </c>
       <c r="U56" s="4">
-        <f>K56*(2^0)+L56*(2^1)+M56*(2^2)+N56*(2^3)+O56*(2^4)+P56*(2^5)+Q56*(2^6)+R56*(2^7)+S56*(2^8)+T56*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V56" s="4"/>
       <c r="W56" s="4">
-        <f>I56+_xlfn.BITLSHIFT(U56,8)</f>
+        <f t="shared" si="24"/>
         <v>160775</v>
       </c>
     </row>
@@ -4410,7 +5592,7 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4">
-        <f>A57*(2^0)+B57*(2^1)+C57*(2^2)+D57*(2^3)+E57*(2^4)+F57*(2^5)+G57*(2^6)+H57*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="J57" s="4"/>
@@ -4445,12 +5627,12 @@
         <v>1</v>
       </c>
       <c r="U57" s="4">
-        <f>K57*(2^0)+L57*(2^1)+M57*(2^2)+N57*(2^3)+O57*(2^4)+P57*(2^5)+Q57*(2^6)+R57*(2^7)+S57*(2^8)+T57*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V57" s="4"/>
       <c r="W57" s="4">
-        <f>I57+_xlfn.BITLSHIFT(U57,8)</f>
+        <f t="shared" si="24"/>
         <v>160776</v>
       </c>
     </row>
@@ -4480,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="4">
-        <f>A58*(2^0)+B58*(2^1)+C58*(2^2)+D58*(2^3)+E58*(2^4)+F58*(2^5)+G58*(2^6)+H58*(2^7)</f>
+        <f t="shared" si="22"/>
         <v>211</v>
       </c>
       <c r="J58" s="4"/>
@@ -4515,12 +5697,12 @@
         <v>1</v>
       </c>
       <c r="U58" s="4">
-        <f>K58*(2^0)+L58*(2^1)+M58*(2^2)+N58*(2^3)+O58*(2^4)+P58*(2^5)+Q58*(2^6)+R58*(2^7)+S58*(2^8)+T58*(2^9)</f>
+        <f t="shared" si="23"/>
         <v>628</v>
       </c>
       <c r="V58" s="4"/>
       <c r="W58" s="4">
-        <f>I58+_xlfn.BITLSHIFT(U58,8)</f>
+        <f t="shared" si="24"/>
         <v>160979</v>
       </c>
     </row>

</xml_diff>